<commit_message>
Add self feedback option and profile icon popup
</commit_message>
<xml_diff>
--- a/server/pending_reviews2.xlsx
+++ b/server/pending_reviews2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>userFeedback</t>
   </si>
@@ -98,8 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -112,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -246,6 +250,64 @@
         <v>45394.229166666664</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="E6" s="0"/>
+      <c r="F6" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="G6" t="n" s="7">
+        <v>45311.229166666664</v>
+      </c>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="K6" s="0"/>
+      <c r="L6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="M6" t="n" s="8">
+        <v>45308.229166666664</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
+      <c r="C7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="E7" s="0"/>
+      <c r="F7" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="G7" t="n" s="9">
+        <v>45311.229166666664</v>
+      </c>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="K7" s="0"/>
+      <c r="L7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="M7" t="n" s="10">
+        <v>45308.229166666664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>